<commit_message>
Screens + modif code mineures
</commit_message>
<xml_diff>
--- a/uml.xlsx
+++ b/uml.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9555" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Modèle" sheetId="1" r:id="rId1"/>
@@ -811,19 +811,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -853,64 +866,63 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -919,18 +931,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1220,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -1234,22 +1234,22 @@
     <row r="1" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="2"/>
       <c r="I2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="2"/>
-      <c r="K2" s="59" t="s">
+      <c r="K2" s="24" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1263,10 +1263,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="38"/>
       <c r="H3" s="2"/>
       <c r="I3" s="10" t="s">
         <v>6</v>
@@ -1286,10 +1286,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="2"/>
       <c r="I4" s="11" t="s">
         <v>7</v>
@@ -1301,16 +1301,16 @@
     </row>
     <row r="5" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1320,16 +1320,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="22"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="K6" t="s">
@@ -1338,34 +1338,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="22"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="K7" s="59" t="s">
+      <c r="K7" s="24" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="22"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="K8" t="s">
@@ -1374,16 +1374,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="K9" t="s">
@@ -1392,16 +1392,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1411,16 +1411,16 @@
     </row>
     <row r="11" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2"/>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1430,28 +1430,28 @@
     </row>
     <row r="12" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="59" t="s">
+      <c r="K12" s="24" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1464,11 +1464,11 @@
     </row>
     <row r="14" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="2"/>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1517,14 +1517,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -1538,6 +1530,14 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1549,7 +1549,7 @@
   <dimension ref="B1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:H9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1563,16 +1563,16 @@
   <sheetData>
     <row r="1" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
-      <c r="F2" s="34" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="F2" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="13" t="s">
@@ -1582,59 +1582,59 @@
       <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="17" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="19" t="s">
         <v>47</v>
       </c>
       <c r="G4" s="12"/>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="19" t="s">
         <v>49</v>
       </c>
       <c r="G5" s="12"/>
-      <c r="H5" s="40" t="s">
+      <c r="H5" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="19" t="s">
         <v>51</v>
       </c>
       <c r="G6" s="12"/>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="20" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1646,186 +1646,208 @@
       <c r="D7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="21" t="s">
         <v>33</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="F8" s="43" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="F8" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="44"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="53"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="F9" s="45" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="F9" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="46"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="F10" s="45" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="F10" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="46"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="F11" s="45" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="F11" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="46"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="48"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="F12" s="45" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
+      <c r="F12" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="46"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="48"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="F13" s="45" t="s">
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="F13" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="46"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="F14" s="45" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="F14" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="46"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="F15" s="45" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+      <c r="F15" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="46"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="F16" s="45" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="F16" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="46"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="48"/>
     </row>
     <row r="17" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="F17" s="45" t="s">
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="F17" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="46"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="48"/>
     </row>
     <row r="18" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="48"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="46"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F19" s="47" t="s">
+      <c r="F19" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="48"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="46"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F20" s="47" t="s">
+      <c r="F20" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="48"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="46"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F21" s="47" t="s">
+      <c r="F21" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="48"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="46"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="48"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="46"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F23" s="47" t="s">
+      <c r="F23" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="48"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="46"/>
     </row>
     <row r="24" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F24" s="49" t="s">
+      <c r="F24" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="50"/>
-      <c r="H24" s="51"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="43"/>
     </row>
     <row r="25" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="F19:H19"/>
@@ -1833,28 +1855,6 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1864,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14:N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1880,446 +1880,434 @@
   <sheetData>
     <row r="3" spans="4:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="4" spans="4:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
-      <c r="H4" s="34" t="s">
+      <c r="E4" s="50"/>
+      <c r="F4" s="51"/>
+      <c r="H4" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="35"/>
-      <c r="J4" s="36"/>
-      <c r="L4" s="34" t="s">
+      <c r="I4" s="50"/>
+      <c r="J4" s="51"/>
+      <c r="L4" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="M4" s="35"/>
-      <c r="N4" s="36"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="51"/>
     </row>
     <row r="5" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="17" t="s">
         <v>71</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="17" t="s">
         <v>71</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="37" t="s">
+      <c r="L5" s="17" t="s">
         <v>71</v>
       </c>
       <c r="M5" s="4"/>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="19" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="19" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="J6" s="40" t="s">
+      <c r="J6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="L6" s="19" t="s">
         <v>92</v>
       </c>
       <c r="M6" s="12"/>
-      <c r="N6" s="40" t="s">
+      <c r="N6" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D7" s="39"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="40"/>
-      <c r="H7" s="39" t="s">
+      <c r="D7" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="53"/>
+      <c r="H7" s="19" t="s">
         <v>78</v>
       </c>
       <c r="I7" s="12"/>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="19" t="s">
         <v>90</v>
       </c>
       <c r="M7" s="12"/>
-      <c r="N7" s="40" t="s">
+      <c r="N7" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="8" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D8" s="39"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="40"/>
-      <c r="H8" s="43" t="s">
+      <c r="D8" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="48"/>
+      <c r="H8" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="I8" s="27"/>
-      <c r="J8" s="44"/>
-      <c r="L8" s="43" t="s">
+      <c r="I8" s="32"/>
+      <c r="J8" s="53"/>
+      <c r="L8" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="M8" s="27"/>
-      <c r="N8" s="44"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="53"/>
     </row>
     <row r="9" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D9" s="39"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="40"/>
-      <c r="H9" s="45" t="s">
+      <c r="D9" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="48"/>
+      <c r="H9" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="46"/>
-      <c r="L9" s="45" t="s">
+      <c r="I9" s="26"/>
+      <c r="J9" s="48"/>
+      <c r="L9" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="21"/>
-      <c r="N9" s="46"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="48"/>
     </row>
     <row r="10" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D10" s="39"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="40"/>
-      <c r="H10" s="45" t="s">
+      <c r="D10" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="48"/>
+      <c r="H10" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="46"/>
-      <c r="L10" s="45" t="s">
+      <c r="I10" s="26"/>
+      <c r="J10" s="48"/>
+      <c r="L10" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="M10" s="21"/>
-      <c r="N10" s="46"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="48"/>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D11" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="44"/>
-      <c r="H11" s="45" t="s">
+      <c r="D11" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="48"/>
+      <c r="H11" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="46"/>
-      <c r="L11" s="45" t="s">
+      <c r="I11" s="26"/>
+      <c r="J11" s="48"/>
+      <c r="L11" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="M11" s="21"/>
-      <c r="N11" s="46"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="48"/>
     </row>
     <row r="12" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="48"/>
+      <c r="H12" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="26"/>
+      <c r="J12" s="48"/>
+      <c r="L12" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="26"/>
+      <c r="N12" s="48"/>
+    </row>
+    <row r="13" spans="4:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D13" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="H13" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="48"/>
+      <c r="L13" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="M13" s="26"/>
+      <c r="N13" s="48"/>
+    </row>
+    <row r="14" spans="4:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="H14" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="26"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="M14" s="26"/>
+      <c r="N14" s="48"/>
+    </row>
+    <row r="15" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="H15" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="45"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="M15" s="45"/>
+      <c r="N15" s="46"/>
+    </row>
+    <row r="16" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="H16" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="45"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="M16" s="55"/>
+      <c r="N16" s="56"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="H17" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="45"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="M17" s="55"/>
+      <c r="N17" s="56"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C18" s="23"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="45"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="M18" s="55"/>
+      <c r="N18" s="56"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C19" s="23"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" s="45"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="M19" s="55"/>
+      <c r="N19" s="56"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C20" s="23"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="45"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="M20" s="55"/>
+      <c r="N20" s="56"/>
+    </row>
+    <row r="21" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C21" s="23"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="I21" s="42"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="54" t="s">
+        <v>86</v>
+      </c>
+      <c r="M21" s="55"/>
+      <c r="N21" s="56"/>
+    </row>
+    <row r="22" spans="3:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C22" s="23"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="46"/>
-      <c r="H12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="46"/>
-      <c r="L12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M12" s="21"/>
-      <c r="N12" s="46"/>
-    </row>
-    <row r="13" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D13" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="46"/>
-      <c r="H13" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="46"/>
-      <c r="L13" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="M13" s="21"/>
-      <c r="N13" s="46"/>
-    </row>
-    <row r="14" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="46"/>
-      <c r="H14" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="M14" s="21"/>
-      <c r="N14" s="46"/>
-    </row>
-    <row r="15" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D15" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="46"/>
-      <c r="H15" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" s="33"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="M15" s="33"/>
-      <c r="N15" s="48"/>
-    </row>
-    <row r="16" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="D16" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="46"/>
-      <c r="H16" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="M16" s="56"/>
-      <c r="N16" s="58"/>
-    </row>
-    <row r="17" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D17" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="54"/>
-      <c r="F17" s="55"/>
-      <c r="H17" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="I17" s="33"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="M17" s="56"/>
-      <c r="N17" s="58"/>
-    </row>
-    <row r="18" spans="3:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="C18" s="52"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="57" t="s">
-        <v>100</v>
-      </c>
-      <c r="M18" s="56"/>
-      <c r="N18" s="58"/>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C19" s="52"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="33"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="M19" s="56"/>
-      <c r="N19" s="58"/>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C20" s="52"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="M20" s="56"/>
-      <c r="N20" s="58"/>
-    </row>
-    <row r="21" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C21" s="52"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="I21" s="50"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="57" t="s">
-        <v>86</v>
-      </c>
-      <c r="M21" s="56"/>
-      <c r="N21" s="58"/>
-    </row>
-    <row r="22" spans="3:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="C22" s="52"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="M22" s="33"/>
-      <c r="N22" s="48"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="46"/>
     </row>
     <row r="23" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C23" s="52"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="49" t="s">
+      <c r="C23" s="23"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="M23" s="50"/>
-      <c r="N23" s="51"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="43"/>
     </row>
     <row r="24" spans="3:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="C24" s="52"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="52"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="23"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C25" s="52"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="52"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="23"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C26" s="52"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="52"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C27" s="52"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="52"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="23"/>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="L17:N17"/>
     <mergeCell ref="L19:N19"/>
     <mergeCell ref="L20:N20"/>
     <mergeCell ref="L21:N21"/>
     <mergeCell ref="L22:N22"/>
     <mergeCell ref="L23:N23"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Principalement le poster TDlog
</commit_message>
<xml_diff>
--- a/uml.xlsx
+++ b/uml.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="114">
   <si>
     <t>Bloc</t>
   </si>
@@ -257,9 +257,6 @@
   </si>
   <si>
     <t>(…)</t>
-  </si>
-  <si>
-    <t>buttonOk</t>
   </si>
   <si>
     <t>compt</t>
@@ -758,7 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -851,6 +848,39 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -866,59 +896,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
@@ -926,6 +908,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -933,30 +957,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1261,23 +1261,23 @@
     <row r="1" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="36"/>
+      <c r="G2" s="47"/>
       <c r="H2" s="2"/>
       <c r="I2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -1290,17 +1290,17 @@
         <v>8</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="38"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="2"/>
       <c r="I3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1313,155 +1313,155 @@
         <v>7</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="2"/>
       <c r="I4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="45"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="45"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="41"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="K6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="41"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="K7" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="41"/>
+      <c r="G8" s="38"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="K8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="41"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="K9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="41"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2"/>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="43"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1469,16 +1469,16 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1486,16 +1486,16 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="2"/>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1503,7 +1503,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
@@ -1515,7 +1515,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
@@ -1527,7 +1527,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="6:7" x14ac:dyDescent="0.45">
@@ -1544,14 +1544,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -1565,6 +1557,14 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1590,16 +1590,16 @@
   <sheetData>
     <row r="1" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
-      <c r="F2" s="50" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="F2" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="62"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="13" t="s">
@@ -1682,177 +1682,199 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="45"/>
-      <c r="F8" s="53" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="44"/>
+      <c r="F8" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="49"/>
-      <c r="H8" s="54"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="64"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
-      <c r="F9" s="55" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="F9" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="56"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="59"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41"/>
-      <c r="F10" s="55" t="s">
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
+      <c r="F10" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="56"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="59"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41"/>
-      <c r="F11" s="55" t="s">
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="F11" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="40"/>
-      <c r="H11" s="56"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="59"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
-      <c r="F12" s="55" t="s">
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="F12" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="56"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="59"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
-      <c r="F13" s="55" t="s">
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="F13" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="56"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="59"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="41"/>
-      <c r="F14" s="55" t="s">
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
+      <c r="F14" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="56"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="41"/>
-      <c r="F15" s="55" t="s">
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="F15" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="40"/>
-      <c r="H15" s="56"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="59"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
-      <c r="F16" s="55" t="s">
+      <c r="C16" s="37"/>
+      <c r="D16" s="38"/>
+      <c r="F16" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="40"/>
-      <c r="H16" s="56"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="59"/>
     </row>
     <row r="17" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="43"/>
-      <c r="F17" s="55" t="s">
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
+      <c r="F17" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="40"/>
-      <c r="H17" s="56"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="59"/>
     </row>
     <row r="18" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="61"/>
-      <c r="H18" s="62"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="57"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F19" s="60" t="s">
+      <c r="F19" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="61"/>
-      <c r="H19" s="62"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="57"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F20" s="60" t="s">
+      <c r="F20" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="61"/>
-      <c r="H20" s="62"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="57"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F21" s="60" t="s">
+      <c r="F21" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="61"/>
-      <c r="H21" s="62"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="57"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="62"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="57"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="F23" s="60" t="s">
+      <c r="F23" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="61"/>
-      <c r="H23" s="62"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="57"/>
     </row>
     <row r="24" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F24" s="57" t="s">
+      <c r="F24" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="58"/>
-      <c r="H24" s="59"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="54"/>
     </row>
     <row r="25" spans="2:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="F19:H19"/>
@@ -1860,28 +1882,6 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1889,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:O34"/>
+  <dimension ref="C3:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1908,30 +1908,30 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="4" spans="3:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="D4" s="50" t="s">
+    <row r="4" spans="3:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="D4" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52"/>
-      <c r="H4" s="50" t="s">
+      <c r="E4" s="61"/>
+      <c r="F4" s="62"/>
+      <c r="H4" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="61"/>
+      <c r="J4" s="62"/>
+      <c r="L4" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="L4" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="52"/>
-    </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="M4" s="61"/>
+      <c r="N4" s="62"/>
+    </row>
+    <row r="5" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D5" s="17" t="s">
         <v>71</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="18" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>71</v>
@@ -1945,335 +1945,335 @@
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="D6" s="32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="19"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="20"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="20"/>
+    </row>
+    <row r="7" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D7" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="33"/>
-      <c r="H6" s="19" t="s">
+      <c r="E7" s="26"/>
+      <c r="F7" s="33"/>
+      <c r="H7" s="19" t="s">
         <v>5</v>
-      </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="D7" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="31"/>
-      <c r="H7" s="19" t="s">
-        <v>78</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="20" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M7" s="25"/>
       <c r="N7" s="20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="D8" s="55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D8" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="31"/>
+      <c r="H8" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="25"/>
+      <c r="J8" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="M8" s="25"/>
+      <c r="N8" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D9" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="56"/>
-      <c r="H8" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I8" s="49"/>
-      <c r="J8" s="54"/>
-      <c r="L8" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="M8" s="49"/>
-      <c r="N8" s="54"/>
-    </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="D9" s="55" t="s">
+      <c r="E9" s="37"/>
+      <c r="F9" s="59"/>
+      <c r="H9" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="43"/>
+      <c r="J9" s="64"/>
+      <c r="L9" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="M9" s="43"/>
+      <c r="N9" s="64"/>
+    </row>
+    <row r="10" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D10" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="56"/>
-      <c r="H9" s="55" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="59"/>
+      <c r="H10" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="40"/>
-      <c r="J9" s="56"/>
-      <c r="L9" s="55" t="s">
+      <c r="I10" s="37"/>
+      <c r="J10" s="59"/>
+      <c r="L10" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="M10" s="37"/>
+      <c r="N10" s="59"/>
+    </row>
+    <row r="11" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D11" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="56"/>
+      <c r="F11" s="57"/>
+      <c r="H11" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="56"/>
+      <c r="J11" s="57"/>
+      <c r="L11" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="M9" s="40"/>
-      <c r="N9" s="56"/>
-    </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="D10" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="61"/>
-      <c r="F10" s="62"/>
-      <c r="H10" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="I10" s="61"/>
-      <c r="J10" s="62"/>
-      <c r="L10" s="55" t="s">
+      <c r="M11" s="37"/>
+      <c r="N11" s="59"/>
+    </row>
+    <row r="12" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D12" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="31"/>
+      <c r="H12" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="56"/>
+      <c r="J12" s="57"/>
+      <c r="L12" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="M10" s="40"/>
-      <c r="N10" s="56"/>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="D11" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="31"/>
-      <c r="H11" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" s="61"/>
-      <c r="J11" s="62"/>
-      <c r="L11" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="M11" s="40"/>
-      <c r="N11" s="56"/>
-    </row>
-    <row r="12" spans="3:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D12" s="63" t="s">
+      <c r="M12" s="37"/>
+      <c r="N12" s="59"/>
+    </row>
+    <row r="13" spans="3:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D13" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="64"/>
-      <c r="F12" s="65"/>
-      <c r="H12" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="I12" s="61"/>
-      <c r="J12" s="62"/>
-      <c r="L12" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="M12" s="40"/>
-      <c r="N12" s="56"/>
-    </row>
-    <row r="13" spans="3:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="E13" s="73"/>
+      <c r="F13" s="74"/>
       <c r="H13" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="56"/>
-      <c r="L13" s="55" t="s">
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
+      <c r="L13" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" s="37"/>
+      <c r="N13" s="59"/>
+    </row>
+    <row r="14" spans="3:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="H14" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="37"/>
+      <c r="J14" s="59"/>
+      <c r="L14" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" s="37"/>
+      <c r="N14" s="59"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="H15" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="56"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="M13" s="40"/>
-      <c r="N13" s="56"/>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="H14" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="I14" s="61"/>
-      <c r="J14" s="62"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="M14" s="28"/>
-      <c r="N14" s="29"/>
-    </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="I15" s="40"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="M15" s="67"/>
-      <c r="N15" s="68"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="29"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C16" s="28"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="56"/>
+      <c r="H16" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="37"/>
+      <c r="J16" s="59"/>
       <c r="K16" s="23"/>
       <c r="L16" s="66" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="M16" s="67"/>
       <c r="N16" s="68"/>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C17" s="28"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="70"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" s="40"/>
-      <c r="J17" s="56"/>
+      <c r="H17" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="37"/>
+      <c r="J17" s="59"/>
       <c r="K17" s="23"/>
       <c r="L17" s="66" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="M17" s="67"/>
       <c r="N17" s="68"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C18" s="28"/>
-      <c r="D18" s="70"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="25"/>
-      <c r="F18" s="70"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="60" t="s">
+      <c r="H18" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="37"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="66" t="s">
         <v>58</v>
-      </c>
-      <c r="I18" s="61"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="66" t="s">
-        <v>97</v>
       </c>
       <c r="M18" s="67"/>
       <c r="N18" s="68"/>
-      <c r="O18" s="28"/>
-    </row>
-    <row r="19" spans="3:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C19" s="28"/>
-      <c r="D19" s="70"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="25"/>
-      <c r="F19" s="70"/>
+      <c r="F19" s="35"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="58"/>
-      <c r="J19" s="59"/>
+      <c r="H19" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="56"/>
+      <c r="J19" s="57"/>
       <c r="K19" s="28"/>
-      <c r="L19" s="60" t="s">
+      <c r="L19" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="M19" s="67"/>
+      <c r="N19" s="68"/>
+      <c r="O19" s="28"/>
+    </row>
+    <row r="20" spans="3:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C20" s="28"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="53"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="M19" s="61"/>
-      <c r="N19" s="62"/>
-      <c r="O19" s="28"/>
-    </row>
-    <row r="20" spans="3:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C20" s="28"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="71" t="s">
-        <v>84</v>
-      </c>
-      <c r="M20" s="72"/>
-      <c r="N20" s="73"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="57"/>
       <c r="O20" s="28"/>
     </row>
-    <row r="21" spans="3:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C21" s="28"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
       <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="L21" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="M21" s="70"/>
+      <c r="N21" s="71"/>
       <c r="O21" s="28"/>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C22" s="28"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
       <c r="K22" s="28"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
       <c r="O22" s="28"/>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C23" s="28"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
       <c r="J23" s="28"/>
       <c r="K23" s="28"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
       <c r="O23" s="28"/>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C24" s="28"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
       <c r="O24" s="28"/>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C25" s="28"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
@@ -2286,9 +2286,9 @@
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C26" s="28"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
@@ -2301,110 +2301,125 @@
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C27" s="28"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
       <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C28" s="28"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="28"/>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C29" s="28"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
       <c r="G29" s="28"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C30" s="28"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="61"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
       <c r="G30" s="28"/>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C31" s="28"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="28"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C32" s="28"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="28"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C33" s="28"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
       <c r="G33" s="28"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="28"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L17:N17"/>
     <mergeCell ref="L18:N18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="L21:N21"/>
     <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L8:N8"/>
     <mergeCell ref="L9:N9"/>
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="L11:N11"/>
     <mergeCell ref="L12:N12"/>
-    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
     <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H18:J18"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>